<commit_message>
add some reports for evosuite
</commit_message>
<xml_diff>
--- a/SF100_900s/35_corina_distribution.xlsx
+++ b/SF100_900s/35_corina_distribution.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="592">
   <si>
     <t>Class</t>
   </si>
@@ -1704,6 +1704,90 @@
   </si>
   <si>
     <t>multiply([[D[[D)[[D</t>
+  </si>
+  <si>
+    <t>scale([[DF)V</t>
+  </si>
+  <si>
+    <t>corina.map.MapFrame</t>
+  </si>
+  <si>
+    <t>corina.map.SiteRenderer</t>
+  </si>
+  <si>
+    <t>drawLabel(Ljava/awt/Graphics2D;Ljava/awt/Point;Lcorina/site/Site;ILcorina/map/View;Ljava/awt/Point;Z)V</t>
+  </si>
+  <si>
+    <t>corina.map.MapPrinter</t>
+  </si>
+  <si>
+    <t>corina.map.PngEncoder</t>
+  </si>
+  <si>
+    <t>setFilter(I)V</t>
+  </si>
+  <si>
+    <t>pngEncode(Z)[B</t>
+  </si>
+  <si>
+    <t>setCompressionLevel(I)V</t>
+  </si>
+  <si>
+    <t>corina.map.LabelSet</t>
+  </si>
+  <si>
+    <t>rehashLocations()V</t>
+  </si>
+  <si>
+    <t>selectAllSites()V</t>
+  </si>
+  <si>
+    <t>showAllSites()V</t>
+  </si>
+  <si>
+    <t>setSelected(Lcorina/site/Site;Z)V</t>
+  </si>
+  <si>
+    <t>setVisible(Lcorina/site/Site;Z)V</t>
+  </si>
+  <si>
+    <t>corina.map.MapPanel</t>
+  </si>
+  <si>
+    <t>setSites(Ljava/util/List;)V</t>
+  </si>
+  <si>
+    <t>updateBuffer()V</t>
+  </si>
+  <si>
+    <t>drawLabel(Ljava/awt/Graphics2D;Ljava/awt/Point;Lcorina/site/Site;ILcorina/map/View;)V</t>
+  </si>
+  <si>
+    <t>setFontForLabel(Ljava/awt/Graphics;Lcorina/map/View;)V</t>
+  </si>
+  <si>
+    <t>siteForPoint(Lcorina/map/Projection;Ljava/awt/Point;I)Lcorina/site/Site;</t>
+  </si>
+  <si>
+    <t>getOffset(Lcorina/site/Location;)Lcorina/map/MapPanel$Offset;</t>
+  </si>
+  <si>
+    <t>corina.map.Layer</t>
+  </si>
+  <si>
+    <t>noDraw()Z</t>
+  </si>
+  <si>
+    <t>update(Lcorina/map/Projection;)V</t>
+  </si>
+  <si>
+    <t>corina.map.PngEncoderB</t>
+  </si>
+  <si>
+    <t>corina.map.layers.SitesLayer</t>
+  </si>
+  <si>
+    <t>drawLabelSR(Ljava/awt/Graphics2D;Ljava/awt/Point;Lcorina/site/Site;ILcorina/map/View;Ljava/awt/Point;Z)V</t>
   </si>
 </sst>
 </file>
@@ -14655,6 +14739,578 @@
         <v>1392376.0</v>
       </c>
     </row>
+    <row r="489">
+      <c r="A489" t="s">
+        <v>562</v>
+      </c>
+      <c r="B489" t="s">
+        <v>564</v>
+      </c>
+      <c r="C489" t="n">
+        <v>1365894.0</v>
+      </c>
+      <c r="D489" t="n">
+        <v>1365898.0</v>
+      </c>
+      <c r="E489" t="n">
+        <v>1365894.0</v>
+      </c>
+      <c r="F489" t="n">
+        <v>1365894.0</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="s">
+        <v>565</v>
+      </c>
+      <c r="B490" t="s">
+        <v>367</v>
+      </c>
+      <c r="C490" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D490" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="s">
+        <v>566</v>
+      </c>
+      <c r="B491" t="s">
+        <v>567</v>
+      </c>
+      <c r="C491" t="n">
+        <v>570.0</v>
+      </c>
+      <c r="D491" t="n">
+        <v>59917.0</v>
+      </c>
+      <c r="E491" t="n">
+        <v>3813.0</v>
+      </c>
+      <c r="F491" t="n">
+        <v>56900.0</v>
+      </c>
+      <c r="G491" t="n">
+        <v>4582.0</v>
+      </c>
+      <c r="H491" t="n">
+        <v>55488.0</v>
+      </c>
+      <c r="I491" t="n">
+        <v>4582.0</v>
+      </c>
+      <c r="J491" t="n">
+        <v>4582.0</v>
+      </c>
+      <c r="K491" t="n">
+        <v>4582.0</v>
+      </c>
+      <c r="L491" t="n">
+        <v>4582.0</v>
+      </c>
+      <c r="M491" t="n">
+        <v>54989.0</v>
+      </c>
+      <c r="N491" t="n">
+        <v>5679.0</v>
+      </c>
+      <c r="O491" t="n">
+        <v>54989.0</v>
+      </c>
+      <c r="P491" t="n">
+        <v>5679.0</v>
+      </c>
+      <c r="Q491" t="n">
+        <v>54989.0</v>
+      </c>
+      <c r="R491" t="n">
+        <v>5679.0</v>
+      </c>
+      <c r="S491" t="n">
+        <v>59908.0</v>
+      </c>
+      <c r="T491" t="n">
+        <v>921.0</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="s">
+        <v>568</v>
+      </c>
+      <c r="B492" t="s">
+        <v>117</v>
+      </c>
+      <c r="C492" t="n">
+        <v>35297.0</v>
+      </c>
+      <c r="D492" t="n">
+        <v>19989.0</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="s">
+        <v>569</v>
+      </c>
+      <c r="B493" t="s">
+        <v>570</v>
+      </c>
+      <c r="C493" t="n">
+        <v>5192873.0</v>
+      </c>
+      <c r="D493" t="n">
+        <v>670678.0</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="s">
+        <v>569</v>
+      </c>
+      <c r="B494" t="s">
+        <v>571</v>
+      </c>
+      <c r="C494" t="n">
+        <v>54835.0</v>
+      </c>
+      <c r="D494" t="n">
+        <v>852496.0</v>
+      </c>
+      <c r="E494" t="n">
+        <v>852326.0</v>
+      </c>
+      <c r="F494" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="s">
+        <v>569</v>
+      </c>
+      <c r="B495" t="s">
+        <v>572</v>
+      </c>
+      <c r="C495" t="n">
+        <v>483107.0</v>
+      </c>
+      <c r="D495" t="n">
+        <v>377865.0</v>
+      </c>
+      <c r="E495" t="n">
+        <v>97043.0</v>
+      </c>
+      <c r="F495" t="n">
+        <v>386284.0</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="s">
+        <v>573</v>
+      </c>
+      <c r="B496" t="s">
+        <v>574</v>
+      </c>
+      <c r="C496" t="n">
+        <v>331461.0</v>
+      </c>
+      <c r="D496" t="n">
+        <v>763945.0</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="s">
+        <v>573</v>
+      </c>
+      <c r="B497" t="s">
+        <v>575</v>
+      </c>
+      <c r="C497" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D497" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E497" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F497" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="s">
+        <v>573</v>
+      </c>
+      <c r="B498" t="s">
+        <v>576</v>
+      </c>
+      <c r="C498" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D498" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E498" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F498" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G498" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H498" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="s">
+        <v>573</v>
+      </c>
+      <c r="B499" t="s">
+        <v>577</v>
+      </c>
+      <c r="C499" t="n">
+        <v>9677.0</v>
+      </c>
+      <c r="D499" t="n">
+        <v>820859.0</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="s">
+        <v>573</v>
+      </c>
+      <c r="B500" t="s">
+        <v>578</v>
+      </c>
+      <c r="C500" t="n">
+        <v>804664.0</v>
+      </c>
+      <c r="D500" t="n">
+        <v>7828.0</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="s">
+        <v>579</v>
+      </c>
+      <c r="B501" t="s">
+        <v>580</v>
+      </c>
+      <c r="C501" t="n">
+        <v>10098.0</v>
+      </c>
+      <c r="D501" t="n">
+        <v>31773.0</v>
+      </c>
+      <c r="E501" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F501" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G501" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H501" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I501" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J501" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="s">
+        <v>579</v>
+      </c>
+      <c r="B502" t="s">
+        <v>581</v>
+      </c>
+      <c r="C502" t="n">
+        <v>41718.0</v>
+      </c>
+      <c r="D502" t="n">
+        <v>41718.0</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="s">
+        <v>579</v>
+      </c>
+      <c r="B503" t="s">
+        <v>582</v>
+      </c>
+      <c r="C503" t="n">
+        <v>7694.0</v>
+      </c>
+      <c r="D503" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="s">
+        <v>579</v>
+      </c>
+      <c r="B504" t="s">
+        <v>583</v>
+      </c>
+      <c r="C504" t="n">
+        <v>50568.0</v>
+      </c>
+      <c r="D504" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="E504" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="F504" t="n">
+        <v>50568.0</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="s">
+        <v>579</v>
+      </c>
+      <c r="B505" t="s">
+        <v>584</v>
+      </c>
+      <c r="C505" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D505" t="n">
+        <v>42929.0</v>
+      </c>
+      <c r="E505" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="F505" t="n">
+        <v>42837.0</v>
+      </c>
+      <c r="G505" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H505" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I505" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J505" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K505" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L505" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M505" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N505" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O505" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P505" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q505" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R505" t="n">
+        <v>42837.0</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="s">
+        <v>579</v>
+      </c>
+      <c r="B506" t="s">
+        <v>557</v>
+      </c>
+      <c r="C506" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D506" t="n">
+        <v>38557.0</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="s">
+        <v>579</v>
+      </c>
+      <c r="B507" t="s">
+        <v>24</v>
+      </c>
+      <c r="C507" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D507" t="n">
+        <v>33855.0</v>
+      </c>
+      <c r="E507" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F507" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G507" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H507" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I507" t="n">
+        <v>20218.0</v>
+      </c>
+      <c r="J507" t="n">
+        <v>20218.0</v>
+      </c>
+      <c r="K507" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="L507" t="n">
+        <v>20218.0</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="s">
+        <v>579</v>
+      </c>
+      <c r="B508" t="s">
+        <v>585</v>
+      </c>
+      <c r="C508" t="n">
+        <v>372.0</v>
+      </c>
+      <c r="D508" t="n">
+        <v>51145.0</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="s">
+        <v>586</v>
+      </c>
+      <c r="B509" t="s">
+        <v>587</v>
+      </c>
+      <c r="C509" t="n">
+        <v>30498.0</v>
+      </c>
+      <c r="D509" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="E509" t="n">
+        <v>30357.0</v>
+      </c>
+      <c r="F509" t="n">
+        <v>141.0</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="s">
+        <v>586</v>
+      </c>
+      <c r="B510" t="s">
+        <v>588</v>
+      </c>
+      <c r="C510" t="n">
+        <v>34395.0</v>
+      </c>
+      <c r="D510" t="n">
+        <v>49872.0</v>
+      </c>
+      <c r="E510" t="n">
+        <v>34322.0</v>
+      </c>
+      <c r="F510" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="G510" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H510" t="n">
+        <v>34322.0</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="s">
+        <v>589</v>
+      </c>
+      <c r="B511" t="s">
+        <v>571</v>
+      </c>
+      <c r="C511" t="n">
+        <v>816994.0</v>
+      </c>
+      <c r="D511" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E511" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F511" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G511" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H511" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="s">
+        <v>590</v>
+      </c>
+      <c r="B512" t="s">
+        <v>580</v>
+      </c>
+      <c r="C512" t="n">
+        <v>135.0</v>
+      </c>
+      <c r="D512" t="n">
+        <v>23102.0</v>
+      </c>
+      <c r="E512" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F512" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G512" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H512" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="s">
+        <v>590</v>
+      </c>
+      <c r="B513" t="s">
+        <v>591</v>
+      </c>
+      <c r="C513" t="n">
+        <v>6094.0</v>
+      </c>
+      <c r="D513" t="n">
+        <v>3549.0</v>
+      </c>
+      <c r="E513" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F513" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>